<commit_message>
Add data from Tape&Media.com. Same code structure as BackupWorks.
</commit_message>
<xml_diff>
--- a/internet_pricing.xlsx
+++ b/internet_pricing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>FUJI</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Tape4Backup</t>
+  </si>
+  <si>
+    <t>Tape&amp;Media</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -451,6 +454,23 @@
         <v>41.15</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>40.86</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1">
+        <v>40.5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tape&Media link fixed. Still works well.
</commit_message>
<xml_diff>
--- a/internet_pricing.xlsx
+++ b/internet_pricing.xlsx
@@ -459,16 +459,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
+        <v>39.44</v>
+      </c>
+      <c r="C4" s="1">
+        <v>39.31</v>
+      </c>
+      <c r="D4" s="1">
+        <v>39.74</v>
+      </c>
+      <c r="E4" s="1">
         <v>40.86</v>
-      </c>
-      <c r="C4" s="1">
-        <v>42</v>
-      </c>
-      <c r="D4" s="1">
-        <v>40.5</v>
-      </c>
-      <c r="E4" s="1">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>